<commit_message>
Added files to analize oscillation histogram
</commit_message>
<xml_diff>
--- a/Oscillazioni/molla.xlsx
+++ b/Oscillazioni/molla.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="864" documentId="13_ncr:1_{19EF7A93-7410-479C-B5A9-9683ABBE8874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3565AC63-C3A7-4159-B49F-7BBAD0D8F809}"/>
+  <xr:revisionPtr revIDLastSave="911" documentId="13_ncr:1_{19EF7A93-7410-479C-B5A9-9683ABBE8874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ED812FC9-2D39-4D4A-9C3B-558B8C837BD0}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Statico - Calibro" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="72">
   <si>
     <t>m [g]</t>
   </si>
@@ -949,7 +949,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1062,6 +1062,13 @@
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -24391,8 +24398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B459E249-CE69-4C2B-8F77-71C2DA9D2D63}">
   <dimension ref="A1:Y18"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="V14" sqref="V14"/>
+    <sheetView topLeftCell="L1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24401,10 +24408,12 @@
     <col min="7" max="7" width="9.140625" customWidth="1"/>
     <col min="10" max="10" width="4.5703125" customWidth="1"/>
     <col min="11" max="11" width="2.28515625" customWidth="1"/>
+    <col min="12" max="13" width="9.140625" customWidth="1"/>
     <col min="14" max="14" width="2.28515625" customWidth="1"/>
     <col min="15" max="15" width="4.5703125" customWidth="1"/>
     <col min="21" max="21" width="4.5703125" customWidth="1"/>
     <col min="22" max="22" width="2.28515625" customWidth="1"/>
+    <col min="23" max="24" width="9.140625" customWidth="1"/>
     <col min="25" max="25" width="2.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -25085,7 +25094,7 @@
   <dimension ref="A1:Y18"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25093,12 +25102,12 @@
     <col min="3" max="4" width="4.5703125" customWidth="1"/>
     <col min="10" max="10" width="4.5703125" customWidth="1"/>
     <col min="11" max="11" width="2.28515625" customWidth="1"/>
-    <col min="13" max="13" width="9" customWidth="1"/>
+    <col min="12" max="13" width="9.140625" customWidth="1"/>
     <col min="14" max="14" width="2.28515625" customWidth="1"/>
     <col min="15" max="15" width="4.5703125" customWidth="1"/>
     <col min="21" max="21" width="4.5703125" customWidth="1"/>
     <col min="22" max="22" width="2.28515625" customWidth="1"/>
-    <col min="24" max="24" width="9" customWidth="1"/>
+    <col min="23" max="24" width="9.140625" customWidth="1"/>
     <col min="25" max="25" width="2.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -25779,7 +25788,7 @@
   <dimension ref="A1:Y21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="V1" sqref="V1:Y9"/>
+      <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25790,6 +25799,7 @@
     <col min="11" max="11" width="9" customWidth="1"/>
     <col min="13" max="13" width="4.5703125" customWidth="1"/>
     <col min="14" max="14" width="2.28515625" customWidth="1"/>
+    <col min="15" max="16" width="9.140625" customWidth="1"/>
     <col min="17" max="17" width="2.28515625" customWidth="1"/>
     <col min="19" max="19" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="10.28515625" bestFit="1" customWidth="1"/>
@@ -25805,7 +25815,7 @@
       <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="51" t="s">
         <v>59</v>
       </c>
       <c r="F1" s="3" t="s">
@@ -25839,18 +25849,10 @@
       <c r="Q1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="V1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="X1" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="Y1" s="3" t="s">
-        <v>60</v>
-      </c>
+      <c r="V1" s="58"/>
+      <c r="W1" s="58"/>
+      <c r="X1" s="58"/>
+      <c r="Y1" s="58"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
@@ -25904,19 +25906,10 @@
       <c r="Q2" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="V2" s="4">
-        <v>19.829999999999998</v>
-      </c>
-      <c r="W2" s="4">
-        <v>0.01</v>
-      </c>
-      <c r="X2" s="6">
-        <v>11.8</v>
-      </c>
-      <c r="Y2" s="6">
-        <f t="shared" ref="Y2:Y9" si="2">POWER(X2,2)*(1/250)/(2*PI())</f>
-        <v>8.8642937104462027E-2</v>
-      </c>
+      <c r="V2" s="59"/>
+      <c r="W2" s="59"/>
+      <c r="X2" s="60"/>
+      <c r="Y2" s="60"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
@@ -25932,7 +25925,7 @@
         <v>9.64</v>
       </c>
       <c r="F3" s="6">
-        <f t="shared" ref="F3:F10" si="3">POWER(E3,2)*(1/250)/(2*PI())</f>
+        <f t="shared" ref="F3:F10" si="2">POWER(E3,2)*(1/250)/(2*PI())</f>
         <v>5.9160820798210396E-2</v>
       </c>
       <c r="H3" s="9">
@@ -25964,19 +25957,10 @@
       <c r="P3" s="13">
         <v>1.3645886683994108</v>
       </c>
-      <c r="V3" s="4">
-        <v>19.78</v>
-      </c>
-      <c r="W3" s="4">
-        <v>0.01</v>
-      </c>
-      <c r="X3" s="6">
-        <v>10.1</v>
-      </c>
-      <c r="Y3" s="6">
-        <f t="shared" si="2"/>
-        <v>6.4941582979216969E-2</v>
-      </c>
+      <c r="V3" s="59"/>
+      <c r="W3" s="59"/>
+      <c r="X3" s="60"/>
+      <c r="Y3" s="60"/>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
@@ -26024,19 +26008,10 @@
       <c r="P4" s="13">
         <v>7</v>
       </c>
-      <c r="V4" s="4">
-        <v>19.760000000000002</v>
-      </c>
-      <c r="W4" s="4">
-        <v>0.01</v>
-      </c>
-      <c r="X4" s="6">
-        <v>9.02</v>
-      </c>
-      <c r="Y4" s="6">
-        <f t="shared" si="2"/>
-        <v>5.1795639327735364E-2</v>
-      </c>
+      <c r="V4" s="59"/>
+      <c r="W4" s="59"/>
+      <c r="X4" s="60"/>
+      <c r="Y4" s="60"/>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
@@ -26052,7 +26027,7 @@
         <v>7.24</v>
       </c>
       <c r="F5" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3.3370080580054931E-2</v>
       </c>
       <c r="H5" s="9">
@@ -26084,19 +26059,10 @@
       <c r="P5" s="13">
         <v>13.034715637468542</v>
       </c>
-      <c r="V5" s="4">
-        <v>19.71</v>
-      </c>
-      <c r="W5" s="4">
-        <v>0.01</v>
-      </c>
-      <c r="X5" s="6">
-        <v>8.2200000000000006</v>
-      </c>
-      <c r="Y5" s="6">
-        <f t="shared" si="2"/>
-        <v>4.3015379427241693E-2</v>
-      </c>
+      <c r="V5" s="59"/>
+      <c r="W5" s="59"/>
+      <c r="X5" s="60"/>
+      <c r="Y5" s="60"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
@@ -26112,7 +26078,7 @@
         <v>6.58</v>
       </c>
       <c r="F6" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2.7563344312335748E-2</v>
       </c>
       <c r="H6" s="9">
@@ -26138,19 +26104,10 @@
       <c r="M6" s="5">
         <v>4</v>
       </c>
-      <c r="V6" s="4">
-        <v>19.78</v>
-      </c>
-      <c r="W6" s="4">
-        <v>0.01</v>
-      </c>
-      <c r="X6" s="6">
-        <v>7.56</v>
-      </c>
-      <c r="Y6" s="6">
-        <f t="shared" si="2"/>
-        <v>3.6385111821987795E-2</v>
-      </c>
+      <c r="V6" s="59"/>
+      <c r="W6" s="59"/>
+      <c r="X6" s="60"/>
+      <c r="Y6" s="60"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
@@ -26166,7 +26123,7 @@
         <v>6.07</v>
       </c>
       <c r="F7" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2.3456191850906302E-2</v>
       </c>
       <c r="H7" s="9">
@@ -26208,19 +26165,10 @@
       </c>
       <c r="T7" s="53"/>
       <c r="U7" s="33"/>
-      <c r="V7" s="4">
-        <v>19.96</v>
-      </c>
-      <c r="W7" s="4">
-        <v>0.01</v>
-      </c>
-      <c r="X7" s="6">
-        <v>7.05</v>
-      </c>
-      <c r="Y7" s="6">
-        <f t="shared" si="2"/>
-        <v>3.1641594236099718E-2</v>
-      </c>
+      <c r="V7" s="59"/>
+      <c r="W7" s="59"/>
+      <c r="X7" s="60"/>
+      <c r="Y7" s="60"/>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
@@ -26236,7 +26184,7 @@
         <v>5.7</v>
       </c>
       <c r="F8" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2.0683776404222722E-2</v>
       </c>
       <c r="H8" s="9">
@@ -26278,19 +26226,10 @@
       </c>
       <c r="T8" s="53"/>
       <c r="U8" s="54"/>
-      <c r="V8" s="4">
-        <v>19.98</v>
-      </c>
-      <c r="W8" s="4">
-        <v>0.01</v>
-      </c>
-      <c r="X8" s="6">
-        <v>6.64</v>
-      </c>
-      <c r="Y8" s="6">
-        <f t="shared" si="2"/>
-        <v>2.8068311115777716E-2</v>
-      </c>
+      <c r="V8" s="59"/>
+      <c r="W8" s="59"/>
+      <c r="X8" s="60"/>
+      <c r="Y8" s="60"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
@@ -26306,7 +26245,7 @@
         <v>5.35</v>
       </c>
       <c r="F9" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1.8221649434591095E-2</v>
       </c>
       <c r="H9" s="9">
@@ -26341,19 +26280,10 @@
       </c>
       <c r="T9" s="53"/>
       <c r="U9" s="53"/>
-      <c r="V9" s="4">
-        <v>19.96</v>
-      </c>
-      <c r="W9" s="4">
-        <v>0.01</v>
-      </c>
-      <c r="X9" s="6">
-        <v>6.29</v>
-      </c>
-      <c r="Y9" s="6">
-        <f t="shared" si="2"/>
-        <v>2.5187288335928228E-2</v>
-      </c>
+      <c r="V9" s="59"/>
+      <c r="W9" s="59"/>
+      <c r="X9" s="60"/>
+      <c r="Y9" s="60"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
@@ -26369,7 +26299,7 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="F10" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1.655848027928079E-2</v>
       </c>
       <c r="H10" s="9">
@@ -26404,10 +26334,10 @@
       </c>
       <c r="T10" s="53"/>
       <c r="U10" s="56"/>
-      <c r="V10" s="4"/>
-      <c r="W10" s="4"/>
-      <c r="X10" s="6"/>
-      <c r="Y10" s="6"/>
+      <c r="V10" s="59"/>
+      <c r="W10" s="59"/>
+      <c r="X10" s="60"/>
+      <c r="Y10" s="60"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
@@ -26473,15 +26403,15 @@
         <v>11.8</v>
       </c>
       <c r="F13" s="6">
-        <f t="shared" ref="F13:F20" si="4">POWER(E13,2)*(1/250)/(2*PI())</f>
+        <f t="shared" ref="F13:F20" si="3">POWER(E13,2)*(1/250)/(2*PI())</f>
         <v>8.8642937104462027E-2</v>
       </c>
       <c r="H13" s="9">
-        <f t="shared" ref="H13:H20" si="5">POWER(E13,-2)</f>
+        <f t="shared" ref="H13:H20" si="4">POWER(E13,-2)</f>
         <v>7.1818442976156272E-3</v>
       </c>
       <c r="I13" s="9">
-        <f t="shared" ref="I13:I20" si="6">2*F13/POWER(E13,3)</f>
+        <f t="shared" ref="I13:I20" si="5">2*F13/POWER(E13,3)</f>
         <v>1.0790165633348835E-4</v>
       </c>
       <c r="J13" s="4">
@@ -26523,15 +26453,15 @@
         <v>10.1</v>
       </c>
       <c r="F14" s="6">
+        <f t="shared" si="3"/>
+        <v>6.4941582979216969E-2</v>
+      </c>
+      <c r="H14" s="9">
         <f t="shared" si="4"/>
-        <v>6.4941582979216969E-2</v>
-      </c>
-      <c r="H14" s="9">
+        <v>9.8029604940692103E-3</v>
+      </c>
+      <c r="I14" s="9">
         <f t="shared" si="5"/>
-        <v>9.8029604940692103E-3</v>
-      </c>
-      <c r="I14" s="9">
-        <f t="shared" si="6"/>
         <v>1.2606332126090719E-4</v>
       </c>
       <c r="J14" s="4">
@@ -26570,15 +26500,15 @@
         <v>9.02</v>
       </c>
       <c r="F15" s="6">
+        <f t="shared" si="3"/>
+        <v>5.1795639327735364E-2</v>
+      </c>
+      <c r="H15" s="9">
         <f t="shared" si="4"/>
-        <v>5.1795639327735364E-2</v>
-      </c>
-      <c r="H15" s="9">
+        <v>1.2290991686373223E-2</v>
+      </c>
+      <c r="I15" s="9">
         <f t="shared" si="5"/>
-        <v>1.2290991686373223E-2</v>
-      </c>
-      <c r="I15" s="9">
-        <f t="shared" si="6"/>
         <v>1.4115737746509566E-4</v>
       </c>
       <c r="J15" s="4">
@@ -26617,15 +26547,15 @@
         <v>8.2200000000000006</v>
       </c>
       <c r="F16" s="6">
+        <f t="shared" si="3"/>
+        <v>4.3015379427241693E-2</v>
+      </c>
+      <c r="H16" s="9">
         <f t="shared" si="4"/>
-        <v>4.3015379427241693E-2</v>
-      </c>
-      <c r="H16" s="9">
+        <v>1.479981766624635E-2</v>
+      </c>
+      <c r="I16" s="9">
         <f t="shared" si="5"/>
-        <v>1.479981766624635E-2</v>
-      </c>
-      <c r="I16" s="9">
-        <f t="shared" si="6"/>
         <v>1.5489532174393708E-4</v>
       </c>
       <c r="J16" s="4">
@@ -26655,15 +26585,15 @@
         <v>7.56</v>
       </c>
       <c r="F17" s="6">
+        <f t="shared" si="3"/>
+        <v>3.6385111821987795E-2</v>
+      </c>
+      <c r="H17" s="9">
         <f t="shared" si="4"/>
-        <v>3.6385111821987795E-2</v>
-      </c>
-      <c r="H17" s="9">
+        <v>1.749671061840374E-2</v>
+      </c>
+      <c r="I17" s="9">
         <f t="shared" si="5"/>
-        <v>1.749671061840374E-2</v>
-      </c>
-      <c r="I17" s="9">
-        <f t="shared" si="6"/>
         <v>1.6841792919777284E-4</v>
       </c>
       <c r="J17" s="4">
@@ -26687,15 +26617,15 @@
         <v>7.05</v>
       </c>
       <c r="F18" s="6">
+        <f t="shared" si="3"/>
+        <v>3.1641594236099718E-2</v>
+      </c>
+      <c r="H18" s="9">
         <f t="shared" si="4"/>
-        <v>3.1641594236099718E-2</v>
-      </c>
-      <c r="H18" s="9">
+        <v>2.011971228811428E-2</v>
+      </c>
+      <c r="I18" s="9">
         <f t="shared" si="5"/>
-        <v>2.011971228811428E-2</v>
-      </c>
-      <c r="I18" s="9">
-        <f t="shared" si="6"/>
         <v>1.8060135386314369E-4</v>
       </c>
       <c r="J18" s="4">
@@ -26735,15 +26665,15 @@
         <v>6.64</v>
       </c>
       <c r="F19" s="6">
+        <f t="shared" si="3"/>
+        <v>2.8068311115777716E-2</v>
+      </c>
+      <c r="H19" s="9">
         <f t="shared" si="4"/>
-        <v>2.8068311115777716E-2</v>
-      </c>
-      <c r="H19" s="9">
+        <v>2.268108578893889E-2</v>
+      </c>
+      <c r="I19" s="9">
         <f t="shared" si="5"/>
-        <v>2.268108578893889E-2</v>
-      </c>
-      <c r="I19" s="9">
-        <f t="shared" si="6"/>
         <v>1.9175294348421128E-4</v>
       </c>
       <c r="J19" s="4">
@@ -26783,15 +26713,15 @@
         <v>6.29</v>
       </c>
       <c r="F20" s="6">
+        <f t="shared" si="3"/>
+        <v>2.5187288335928228E-2</v>
+      </c>
+      <c r="H20" s="9">
         <f t="shared" si="4"/>
-        <v>2.5187288335928228E-2</v>
-      </c>
-      <c r="H20" s="9">
+        <v>2.527543909756572E-2</v>
+      </c>
+      <c r="I20" s="9">
         <f t="shared" si="5"/>
-        <v>2.527543909756572E-2</v>
-      </c>
-      <c r="I20" s="9">
-        <f t="shared" si="6"/>
         <v>2.024228211025696E-4</v>
       </c>
       <c r="J20" s="4">

</xml_diff>